<commit_message>
Remove parenthesized unit names from SITs (e.g. KZI "CV (CVS)" -> "CV").
</commit_message>
<xml_diff>
--- a/sits/msit_hydrans.xlsx
+++ b/sits/msit_hydrans.xlsx
@@ -204,7 +204,7 @@
     <t>Heavy Carrier Group</t>
   </si>
   <si>
-    <t>ID (CVA)</t>
+    <t>ID</t>
   </si>
   <si>
     <t>10-12(12)/5-6(6)</t>
@@ -4998,8 +4998,8 @@
   </sheetPr>
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A190" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H198" activeCellId="0" pane="topLeft" sqref="H198"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add HYD LC to SITs.
</commit_message>
<xml_diff>
--- a/sits/msit_hydrans.xlsx
+++ b/sits/msit_hydrans.xlsx
@@ -4998,8 +4998,8 @@
   </sheetPr>
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D24" activeCellId="0" pane="topLeft" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5717,7 +5717,7 @@
         <v>120</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E24" s="7" t="n">
         <v>9</v>

</xml_diff>

<commit_message>
Modify one of the HYD LM counters to be a LC, and fix stats for LM and LC in SITs.
</commit_message>
<xml_diff>
--- a/sits/msit_hydrans.xlsx
+++ b/sits/msit_hydrans.xlsx
@@ -408,7 +408,26 @@
     <t>LC</t>
   </si>
   <si>
-    <t>7-9(3)/5(1)</t>
+    <r>
+      <t xml:space="preserve">7-9(3)/5(1</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">▲</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val=""/>
+        <charset val="1"/>
+        <family val="1"/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>From RN: 2
@@ -461,7 +480,26 @@
     <t>LM</t>
   </si>
   <si>
-    <t>8-9(3)/5(1)</t>
+    <r>
+      <t xml:space="preserve">8-9(3)/5(1</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">▲</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val=""/>
+        <charset val="1"/>
+        <family val="1"/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>Y159</t>
@@ -4531,7 +4569,7 @@
     <numFmt formatCode="###0.00;###0.00" numFmtId="167"/>
     <numFmt formatCode="###0.000;###0.000" numFmtId="168"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <name val="Times New Roman"/>
       <charset val="204"/>
@@ -4584,6 +4622,17 @@
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val=""/>
+      <charset val="1"/>
+      <family val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="MS Gothic"/>
+      <family val="3"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -4674,7 +4723,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -4799,7 +4848,15 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="167" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4998,8 +5055,8 @@
   </sheetPr>
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D24" activeCellId="0" pane="topLeft" sqref="D24"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C24" activeCellId="0" pane="topLeft" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5713,7 +5770,7 @@
       <c r="B24" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="31" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -5734,7 +5791,7 @@
       <c r="I24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="31" t="n">
+      <c r="J24" s="32" t="n">
         <v>2.25</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -5853,7 +5910,7 @@
       <c r="B28" s="26" t="n">
         <v>19</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="33" t="s">
         <v>137</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -5874,7 +5931,7 @@
       <c r="I28" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="J28" s="32" t="n">
+      <c r="J28" s="34" t="n">
         <v>2.25</v>
       </c>
       <c r="K28" s="19" t="s">
@@ -5909,7 +5966,7 @@
       <c r="I29" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="J29" s="32" t="n">
+      <c r="J29" s="34" t="n">
         <v>2.25</v>
       </c>
       <c r="K29" s="19" t="s">
@@ -6022,34 +6079,34 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="33">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="35" t="n">
+      <c r="E33" s="37" t="n">
         <v>8</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="33" t="s">
+      <c r="G33" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="H33" s="33" t="s">
+      <c r="H33" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="I33" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="J33" s="36" t="n">
+      <c r="J33" s="38" t="n">
         <v>2</v>
       </c>
       <c r="K33" s="9" t="s">
@@ -6063,7 +6120,7 @@
       <c r="B34" s="23" t="n">
         <v>68</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="39" t="s">
         <v>169</v>
       </c>
       <c r="D34" s="21" t="s">
@@ -6098,7 +6155,7 @@
       <c r="B35" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="40" t="s">
         <v>174</v>
       </c>
       <c r="D35" s="19" t="s">
@@ -6154,7 +6211,7 @@
       <c r="I36" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="J36" s="39" t="n">
+      <c r="J36" s="41" t="n">
         <v>2</v>
       </c>
       <c r="K36" s="9" t="s">
@@ -6224,7 +6281,7 @@
       <c r="I38" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J38" s="31" t="n">
+      <c r="J38" s="32" t="n">
         <v>2.25</v>
       </c>
       <c r="K38" s="4" t="s">
@@ -6238,7 +6295,7 @@
       <c r="B39" s="26" t="n">
         <v>116</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="39" t="s">
         <v>194</v>
       </c>
       <c r="D39" s="19" t="s">
@@ -6259,7 +6316,7 @@
       <c r="I39" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="J39" s="32" t="n">
+      <c r="J39" s="34" t="n">
         <v>2.25</v>
       </c>
       <c r="K39" s="19" t="s">
@@ -6364,7 +6421,7 @@
       <c r="I42" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="J42" s="40" t="n">
+      <c r="J42" s="42" t="n">
         <v>3.25</v>
       </c>
       <c r="K42" s="11" t="s">
@@ -6498,7 +6555,7 @@
       <c r="B47" s="26" t="n">
         <v>93</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="40" t="s">
         <v>234</v>
       </c>
       <c r="D47" s="19" t="s">
@@ -6519,7 +6576,7 @@
       <c r="I47" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="J47" s="32" t="n">
+      <c r="J47" s="34" t="n">
         <v>1.75</v>
       </c>
       <c r="K47" s="19" t="s">
@@ -6568,7 +6625,7 @@
       <c r="B49" s="26" t="n">
         <v>96</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="40" t="s">
         <v>239</v>
       </c>
       <c r="D49" s="19" t="s">
@@ -6603,7 +6660,7 @@
       <c r="B50" s="26" t="n">
         <v>101</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="40" t="s">
         <v>244</v>
       </c>
       <c r="D50" s="19" t="s">
@@ -6624,7 +6681,7 @@
       <c r="I50" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="J50" s="32" t="n">
+      <c r="J50" s="34" t="n">
         <v>1.5</v>
       </c>
       <c r="K50" s="21" t="s">
@@ -6659,7 +6716,7 @@
       <c r="I51" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="J51" s="31" t="n">
+      <c r="J51" s="32" t="n">
         <v>1.75</v>
       </c>
       <c r="K51" s="4" t="s">
@@ -6694,7 +6751,7 @@
       <c r="I52" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="J52" s="31" t="n">
+      <c r="J52" s="32" t="n">
         <v>1.5</v>
       </c>
       <c r="K52" s="11" t="s">
@@ -6708,7 +6765,7 @@
       <c r="B53" s="16" t="n">
         <v>97</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="43" t="s">
         <v>259</v>
       </c>
       <c r="D53" s="15" t="s">
@@ -6740,31 +6797,31 @@
       <c r="A54" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="44" t="s">
         <v>263</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="44" t="n">
+      <c r="E54" s="46" t="n">
         <v>8</v>
       </c>
-      <c r="F54" s="42" t="s">
+      <c r="F54" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="G54" s="42" t="s">
+      <c r="G54" s="44" t="s">
         <v>219</v>
       </c>
       <c r="H54" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="I54" s="42" t="s">
+      <c r="I54" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="J54" s="45" t="n">
+      <c r="J54" s="47" t="n">
         <v>1.5</v>
       </c>
       <c r="K54" s="19" t="s">
@@ -6772,72 +6829,72 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="53" outlineLevel="0" r="55">
-      <c r="A55" s="42" t="s">
+      <c r="A55" s="44" t="s">
         <v>268</v>
       </c>
-      <c r="B55" s="46" t="n">
+      <c r="B55" s="48" t="n">
         <v>100</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C55" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="D55" s="42" t="s">
+      <c r="D55" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="44" t="n">
+      <c r="E55" s="46" t="n">
         <v>8</v>
       </c>
-      <c r="F55" s="42" t="s">
+      <c r="F55" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="G55" s="42" t="s">
+      <c r="G55" s="44" t="s">
         <v>219</v>
       </c>
       <c r="H55" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="I55" s="42" t="s">
+      <c r="I55" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="J55" s="45" t="n">
+      <c r="J55" s="47" t="n">
         <v>1.5</v>
       </c>
-      <c r="K55" s="42" t="s">
+      <c r="K55" s="44" t="s">
         <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="75" outlineLevel="0" r="56">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="44" t="s">
         <v>273</v>
       </c>
-      <c r="B56" s="46" t="n">
+      <c r="B56" s="48" t="n">
         <v>102</v>
       </c>
-      <c r="C56" s="43" t="s">
+      <c r="C56" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="D56" s="42" t="s">
+      <c r="D56" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="E56" s="44" t="n">
+      <c r="E56" s="46" t="n">
         <v>8</v>
       </c>
-      <c r="F56" s="42" t="s">
+      <c r="F56" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="G56" s="42" t="s">
+      <c r="G56" s="44" t="s">
         <v>219</v>
       </c>
       <c r="H56" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="I56" s="42" t="s">
+      <c r="I56" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="J56" s="47" t="n">
+      <c r="J56" s="49" t="n">
         <v>1.5</v>
       </c>
-      <c r="K56" s="42" t="s">
+      <c r="K56" s="44" t="s">
         <v>277</v>
       </c>
     </row>
@@ -6848,7 +6905,7 @@
       <c r="B57" s="5" t="n">
         <v>95</v>
       </c>
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="50" t="s">
         <v>279</v>
       </c>
       <c r="D57" s="4" t="s">
@@ -6883,7 +6940,7 @@
       <c r="B58" s="16" t="n">
         <v>99</v>
       </c>
-      <c r="C58" s="49" t="s">
+      <c r="C58" s="51" t="s">
         <v>284</v>
       </c>
       <c r="D58" s="15" t="s">
@@ -6904,7 +6961,7 @@
       <c r="I58" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="J58" s="50" t="n">
+      <c r="J58" s="52" t="n">
         <v>1.5</v>
       </c>
       <c r="K58" s="4" t="s">
@@ -6918,7 +6975,7 @@
       <c r="B59" s="26" t="n">
         <v>98</v>
       </c>
-      <c r="C59" s="38" t="s">
+      <c r="C59" s="40" t="s">
         <v>289</v>
       </c>
       <c r="D59" s="19" t="s">
@@ -6947,19 +7004,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="60">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="53" t="s">
         <v>293</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="51"/>
-      <c r="K60" s="51"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="61">
       <c r="A61" s="1" t="s">
@@ -7024,7 +7081,7 @@
       <c r="I62" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="J62" s="31" t="n">
+      <c r="J62" s="32" t="n">
         <v>1.75</v>
       </c>
       <c r="K62" s="4" t="s">
@@ -7059,7 +7116,7 @@
       <c r="I63" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="J63" s="31" t="n">
+      <c r="J63" s="32" t="n">
         <v>1.75</v>
       </c>
       <c r="K63" s="4" t="s">
@@ -7094,7 +7151,7 @@
       <c r="I64" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="J64" s="31" t="n">
+      <c r="J64" s="32" t="n">
         <v>1.75</v>
       </c>
       <c r="K64" s="4" t="s">
@@ -7108,7 +7165,7 @@
       <c r="B65" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="C65" s="39" t="s">
         <v>316</v>
       </c>
       <c r="D65" s="19" t="s">
@@ -7129,7 +7186,7 @@
       <c r="I65" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="J65" s="32" t="n">
+      <c r="J65" s="34" t="n">
         <v>1.75</v>
       </c>
       <c r="K65" s="19" t="s">
@@ -7164,7 +7221,7 @@
       <c r="I66" s="21" t="s">
         <v>321</v>
       </c>
-      <c r="J66" s="52" t="n">
+      <c r="J66" s="54" t="n">
         <v>1.75</v>
       </c>
       <c r="K66" s="21" t="s">
@@ -7178,7 +7235,7 @@
       <c r="B67" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="C67" s="39" t="s">
         <v>325</v>
       </c>
       <c r="D67" s="21" t="s">
@@ -7199,7 +7256,7 @@
       <c r="I67" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="J67" s="52" t="n">
+      <c r="J67" s="54" t="n">
         <v>1.75</v>
       </c>
       <c r="K67" s="21" t="s">
@@ -7234,7 +7291,7 @@
       <c r="I68" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="J68" s="31" t="n">
+      <c r="J68" s="32" t="n">
         <v>1.75</v>
       </c>
       <c r="K68" s="4" t="s">
@@ -7269,7 +7326,7 @@
       <c r="I69" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="J69" s="40" t="n">
+      <c r="J69" s="42" t="n">
         <v>1.75</v>
       </c>
       <c r="K69" s="11" t="s">
@@ -7319,7 +7376,7 @@
       <c r="I71" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="J71" s="40" t="n">
+      <c r="J71" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K71" s="11" t="s">
@@ -7333,7 +7390,7 @@
       <c r="B72" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="C72" s="50" t="s">
         <v>348</v>
       </c>
       <c r="D72" s="11" t="s">
@@ -7354,7 +7411,7 @@
       <c r="I72" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="J72" s="40" t="n">
+      <c r="J72" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K72" s="11" t="s">
@@ -7389,7 +7446,7 @@
       <c r="I73" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="J73" s="31" t="n">
+      <c r="J73" s="32" t="n">
         <v>1.25</v>
       </c>
       <c r="K73" s="4" t="s">
@@ -7403,7 +7460,7 @@
       <c r="B74" s="26" t="n">
         <v>36</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="39" t="s">
         <v>358</v>
       </c>
       <c r="D74" s="19" t="s">
@@ -7424,7 +7481,7 @@
       <c r="I74" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="J74" s="32" t="n">
+      <c r="J74" s="34" t="n">
         <v>1.25</v>
       </c>
       <c r="K74" s="19" t="s">
@@ -7459,7 +7516,7 @@
       <c r="I75" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="J75" s="32" t="n">
+      <c r="J75" s="34" t="n">
         <v>1.25</v>
       </c>
       <c r="K75" s="19" t="s">
@@ -7494,7 +7551,7 @@
       <c r="I76" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="J76" s="32" t="n">
+      <c r="J76" s="34" t="n">
         <v>1.25</v>
       </c>
       <c r="K76" s="19" t="s">
@@ -7564,7 +7621,7 @@
       <c r="I78" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="J78" s="31" t="n">
+      <c r="J78" s="32" t="n">
         <v>1.25</v>
       </c>
       <c r="K78" s="4" t="s">
@@ -7578,7 +7635,7 @@
       <c r="B79" s="14" t="n">
         <v>114</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="55" t="s">
         <v>381</v>
       </c>
       <c r="D79" s="11" t="s">
@@ -7599,7 +7656,7 @@
       <c r="I79" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="J79" s="40" t="n">
+      <c r="J79" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K79" s="11" t="s">
@@ -7698,7 +7755,7 @@
       <c r="I82" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="J82" s="32" t="n">
+      <c r="J82" s="34" t="n">
         <v>1.25</v>
       </c>
       <c r="K82" s="19" t="s">
@@ -7712,7 +7769,7 @@
       <c r="B83" s="16" t="n">
         <v>89</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="51" t="s">
         <v>395</v>
       </c>
       <c r="D83" s="15" t="s">
@@ -7733,7 +7790,7 @@
       <c r="I83" s="15" t="s">
         <v>397</v>
       </c>
-      <c r="J83" s="50" t="n">
+      <c r="J83" s="52" t="n">
         <v>1.25</v>
       </c>
       <c r="K83" s="4" t="s">
@@ -7768,7 +7825,7 @@
       <c r="I84" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="J84" s="40" t="n">
+      <c r="J84" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K84" s="11" t="s">
@@ -7776,19 +7833,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="85">
-      <c r="A85" s="51" t="s">
+      <c r="A85" s="53" t="s">
         <v>403</v>
       </c>
-      <c r="B85" s="51"/>
-      <c r="C85" s="51"/>
-      <c r="D85" s="51"/>
-      <c r="E85" s="51"/>
-      <c r="F85" s="51"/>
-      <c r="G85" s="51"/>
-      <c r="H85" s="51"/>
-      <c r="I85" s="51"/>
-      <c r="J85" s="51"/>
-      <c r="K85" s="51"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="53"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="53"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="86">
       <c r="A86" s="1" t="s">
@@ -7853,7 +7910,7 @@
       <c r="I87" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="J87" s="54" t="n">
+      <c r="J87" s="56" t="n">
         <v>2</v>
       </c>
       <c r="K87" s="9" t="s">
@@ -7888,7 +7945,7 @@
       <c r="I88" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="J88" s="54" t="n">
+      <c r="J88" s="56" t="n">
         <v>3.5</v>
       </c>
       <c r="K88" s="9" t="s">
@@ -7938,7 +7995,7 @@
       <c r="I90" s="15" t="s">
         <v>420</v>
       </c>
-      <c r="J90" s="50" t="n">
+      <c r="J90" s="52" t="n">
         <v>1.25</v>
       </c>
       <c r="K90" s="4" t="s">
@@ -7973,7 +8030,7 @@
       <c r="I91" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="J91" s="40" t="n">
+      <c r="J91" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K91" s="11" t="s">
@@ -8008,7 +8065,7 @@
       <c r="I92" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="J92" s="40" t="n">
+      <c r="J92" s="42" t="n">
         <v>1.25</v>
       </c>
       <c r="K92" s="11" t="s">
@@ -8142,7 +8199,7 @@
       <c r="B97" s="24" t="n">
         <v>9</v>
       </c>
-      <c r="C97" s="55" t="s">
+      <c r="C97" s="57" t="s">
         <v>449</v>
       </c>
       <c r="D97" s="21" t="s">
@@ -8177,7 +8234,7 @@
       <c r="B98" s="19" t="s">
         <v>454</v>
       </c>
-      <c r="C98" s="38" t="s">
+      <c r="C98" s="40" t="s">
         <v>455</v>
       </c>
       <c r="D98" s="19" t="s">
@@ -8212,7 +8269,7 @@
       <c r="B99" s="19" t="s">
         <v>461</v>
       </c>
-      <c r="C99" s="38" t="s">
+      <c r="C99" s="40" t="s">
         <v>462</v>
       </c>
       <c r="D99" s="19" t="s">
@@ -8352,7 +8409,7 @@
       <c r="B103" s="26" t="n">
         <v>71</v>
       </c>
-      <c r="C103" s="37" t="s">
+      <c r="C103" s="39" t="s">
         <v>443</v>
       </c>
       <c r="D103" s="19" t="s">
@@ -8422,7 +8479,7 @@
       <c r="B105" s="26" t="n">
         <v>72</v>
       </c>
-      <c r="C105" s="38" t="s">
+      <c r="C105" s="40" t="s">
         <v>487</v>
       </c>
       <c r="D105" s="19" t="s">
@@ -8478,7 +8535,7 @@
       <c r="I106" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="J106" s="40" t="n">
+      <c r="J106" s="42" t="n">
         <v>2.25</v>
       </c>
       <c r="K106" s="11" t="s">
@@ -8492,7 +8549,7 @@
       <c r="B107" s="16" t="n">
         <v>206</v>
       </c>
-      <c r="C107" s="49" t="s">
+      <c r="C107" s="51" t="s">
         <v>497</v>
       </c>
       <c r="D107" s="15" t="s">
@@ -8513,7 +8570,7 @@
       <c r="I107" s="15" t="s">
         <v>499</v>
       </c>
-      <c r="J107" s="50" t="n">
+      <c r="J107" s="52" t="n">
         <v>2.25</v>
       </c>
       <c r="K107" s="15" t="s">
@@ -8562,7 +8619,7 @@
       <c r="B109" s="14" t="n">
         <v>205</v>
       </c>
-      <c r="C109" s="48" t="s">
+      <c r="C109" s="50" t="s">
         <v>502</v>
       </c>
       <c r="D109" s="11" t="s">
@@ -8583,7 +8640,7 @@
       <c r="I109" s="11" t="s">
         <v>504</v>
       </c>
-      <c r="J109" s="40" t="n">
+      <c r="J109" s="42" t="n">
         <v>2.25</v>
       </c>
       <c r="K109" s="11" t="s">
@@ -8711,72 +8768,72 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="114">
-      <c r="A114" s="42" t="s">
+      <c r="A114" s="44" t="s">
         <v>521</v>
       </c>
-      <c r="B114" s="46" t="n">
+      <c r="B114" s="48" t="n">
         <v>78</v>
       </c>
-      <c r="C114" s="38" t="s">
+      <c r="C114" s="40" t="s">
         <v>522</v>
       </c>
-      <c r="D114" s="42" t="s">
+      <c r="D114" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E114" s="44" t="n">
+      <c r="E114" s="46" t="n">
         <v>5</v>
       </c>
-      <c r="F114" s="42" t="s">
+      <c r="F114" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="G114" s="42" t="s">
+      <c r="G114" s="44" t="s">
         <v>508</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>523</v>
       </c>
-      <c r="I114" s="42" t="s">
+      <c r="I114" s="44" t="s">
         <v>524</v>
       </c>
-      <c r="J114" s="45" t="n">
+      <c r="J114" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="K114" s="42" t="s">
+      <c r="K114" s="44" t="s">
         <v>525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="115">
-      <c r="A115" s="42" t="s">
+      <c r="A115" s="44" t="s">
         <v>526</v>
       </c>
-      <c r="B115" s="46" t="n">
+      <c r="B115" s="48" t="n">
         <v>76</v>
       </c>
-      <c r="C115" s="42" t="s">
+      <c r="C115" s="44" t="s">
         <v>527</v>
       </c>
-      <c r="D115" s="42" t="s">
+      <c r="D115" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E115" s="44" t="n">
+      <c r="E115" s="46" t="n">
         <v>6</v>
       </c>
-      <c r="F115" s="42" t="s">
+      <c r="F115" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="G115" s="42" t="s">
+      <c r="G115" s="44" t="s">
         <v>508</v>
       </c>
       <c r="H115" s="21" t="s">
         <v>528</v>
       </c>
-      <c r="I115" s="42" t="s">
+      <c r="I115" s="44" t="s">
         <v>529</v>
       </c>
-      <c r="J115" s="45" t="n">
+      <c r="J115" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="K115" s="42" t="s">
+      <c r="K115" s="44" t="s">
         <v>530</v>
       </c>
     </row>
@@ -8787,7 +8844,7 @@
       <c r="B116" s="16" t="n">
         <v>79</v>
       </c>
-      <c r="C116" s="49" t="s">
+      <c r="C116" s="51" t="s">
         <v>532</v>
       </c>
       <c r="D116" s="15" t="s">
@@ -8872,7 +8929,7 @@
       <c r="B119" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="C119" s="48" t="s">
+      <c r="C119" s="50" t="s">
         <v>543</v>
       </c>
       <c r="D119" s="11" t="s">
@@ -8893,7 +8950,7 @@
       <c r="I119" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="J119" s="56" t="n">
+      <c r="J119" s="58" t="n">
         <v>0.625</v>
       </c>
       <c r="K119" s="11" t="s">
@@ -8928,7 +8985,7 @@
       <c r="I120" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="J120" s="56" t="n">
+      <c r="J120" s="58" t="n">
         <v>0.625</v>
       </c>
       <c r="K120" s="11" t="s">
@@ -8963,7 +9020,7 @@
       <c r="I121" s="11" t="s">
         <v>556</v>
       </c>
-      <c r="J121" s="56" t="n">
+      <c r="J121" s="58" t="n">
         <v>0.625</v>
       </c>
       <c r="K121" s="11" t="s">
@@ -8998,7 +9055,7 @@
       <c r="I122" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="J122" s="57" t="n">
+      <c r="J122" s="59" t="n">
         <v>0.625</v>
       </c>
       <c r="K122" s="19" t="s">
@@ -9012,7 +9069,7 @@
       <c r="B123" s="23" t="n">
         <v>41</v>
       </c>
-      <c r="C123" s="55" t="s">
+      <c r="C123" s="57" t="s">
         <v>563</v>
       </c>
       <c r="D123" s="21" t="s">
@@ -9033,7 +9090,7 @@
       <c r="I123" s="21" t="s">
         <v>551</v>
       </c>
-      <c r="J123" s="58" t="n">
+      <c r="J123" s="60" t="n">
         <v>0.875</v>
       </c>
       <c r="K123" s="21" t="s">
@@ -9047,7 +9104,7 @@
       <c r="B124" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="C124" s="55" t="s">
+      <c r="C124" s="57" t="s">
         <v>566</v>
       </c>
       <c r="D124" s="21" t="s">
@@ -9068,7 +9125,7 @@
       <c r="I124" s="21" t="s">
         <v>546</v>
       </c>
-      <c r="J124" s="58" t="n">
+      <c r="J124" s="60" t="n">
         <v>0.625</v>
       </c>
       <c r="K124" s="21" t="s">
@@ -9082,7 +9139,7 @@
       <c r="B125" s="23" t="n">
         <v>69</v>
       </c>
-      <c r="C125" s="37" t="s">
+      <c r="C125" s="39" t="s">
         <v>570</v>
       </c>
       <c r="D125" s="21" t="s">
@@ -9103,7 +9160,7 @@
       <c r="I125" s="21" t="s">
         <v>572</v>
       </c>
-      <c r="J125" s="58" t="n">
+      <c r="J125" s="60" t="n">
         <v>0.625</v>
       </c>
       <c r="K125" s="21" t="s">
@@ -9138,7 +9195,7 @@
       <c r="I126" s="11" t="s">
         <v>576</v>
       </c>
-      <c r="J126" s="56" t="n">
+      <c r="J126" s="58" t="n">
         <v>0.625</v>
       </c>
       <c r="K126" s="11" t="s">
@@ -9173,7 +9230,7 @@
       <c r="I127" s="11" t="s">
         <v>572</v>
       </c>
-      <c r="J127" s="56" t="n">
+      <c r="J127" s="58" t="n">
         <v>0.625</v>
       </c>
       <c r="K127" s="11" t="s">
@@ -9475,27 +9532,27 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="138">
-      <c r="A138" s="33" t="s">
+      <c r="A138" s="35" t="s">
         <v>613</v>
       </c>
-      <c r="B138" s="59" t="n">
+      <c r="B138" s="61" t="n">
         <v>112</v>
       </c>
       <c r="C138" s="10"/>
-      <c r="D138" s="33" t="s">
+      <c r="D138" s="35" t="s">
         <v>607</v>
       </c>
-      <c r="E138" s="35" t="n">
+      <c r="E138" s="37" t="n">
         <v>8</v>
       </c>
       <c r="F138" s="10"/>
-      <c r="G138" s="33" t="s">
+      <c r="G138" s="35" t="s">
         <v>608</v>
       </c>
-      <c r="H138" s="33" t="s">
+      <c r="H138" s="35" t="s">
         <v>614</v>
       </c>
-      <c r="I138" s="33" t="s">
+      <c r="I138" s="35" t="s">
         <v>615</v>
       </c>
       <c r="J138" s="10"/>
@@ -9627,7 +9684,7 @@
       <c r="A143" s="21" t="s">
         <v>633</v>
       </c>
-      <c r="B143" s="55" t="s">
+      <c r="B143" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C143" s="21" t="s">
@@ -9805,7 +9862,7 @@
       <c r="B148" s="26" t="n">
         <v>28</v>
       </c>
-      <c r="C148" s="37" t="s">
+      <c r="C148" s="39" t="s">
         <v>658</v>
       </c>
       <c r="D148" s="19" t="s">
@@ -9925,7 +9982,7 @@
       <c r="B152" s="11" t="s">
         <v>667</v>
       </c>
-      <c r="C152" s="48" t="s">
+      <c r="C152" s="50" t="s">
         <v>17</v>
       </c>
       <c r="D152" s="11" t="s">
@@ -10066,7 +10123,7 @@
       <c r="I156" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="J156" s="31" t="n">
+      <c r="J156" s="32" t="n">
         <v>0.75</v>
       </c>
       <c r="K156" s="4" t="s">
@@ -10302,7 +10359,7 @@
       <c r="B165" s="21" t="s">
         <v>712</v>
       </c>
-      <c r="C165" s="37" t="s">
+      <c r="C165" s="39" t="s">
         <v>713</v>
       </c>
       <c r="D165" s="21" t="s">
@@ -10442,7 +10499,7 @@
       <c r="B169" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="C169" s="49" t="s">
+      <c r="C169" s="51" t="s">
         <v>734</v>
       </c>
       <c r="D169" s="4" t="s">
@@ -10927,7 +10984,7 @@
       <c r="B184" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="C184" s="53" t="s">
+      <c r="C184" s="55" t="s">
         <v>800</v>
       </c>
       <c r="D184" s="4" t="s">
@@ -11272,7 +11329,7 @@
       <c r="B195" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C195" s="49" t="s">
+      <c r="C195" s="51" t="s">
         <v>842</v>
       </c>
       <c r="D195" s="4" t="s">
@@ -11307,7 +11364,7 @@
       <c r="B196" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="C196" s="53" t="s">
+      <c r="C196" s="55" t="s">
         <v>634</v>
       </c>
       <c r="D196" s="11" t="s">
@@ -11342,7 +11399,7 @@
       <c r="B197" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="C197" s="53" t="s">
+      <c r="C197" s="55" t="s">
         <v>850</v>
       </c>
       <c r="D197" s="11" t="s">
@@ -11377,7 +11434,7 @@
       <c r="B198" s="4" t="s">
         <v>853</v>
       </c>
-      <c r="C198" s="53" t="s">
+      <c r="C198" s="55" t="s">
         <v>854</v>
       </c>
       <c r="D198" s="4" t="s">
@@ -11398,7 +11455,7 @@
       <c r="I198" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="J198" s="31" t="n">
+      <c r="J198" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K198" s="11" t="s">
@@ -11412,7 +11469,7 @@
       <c r="B199" s="21" t="s">
         <v>636</v>
       </c>
-      <c r="C199" s="55" t="s">
+      <c r="C199" s="57" t="s">
         <v>860</v>
       </c>
       <c r="D199" s="21" t="s">
@@ -11517,7 +11574,7 @@
       <c r="B202" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="C202" s="48" t="s">
+      <c r="C202" s="50" t="s">
         <v>873</v>
       </c>
       <c r="D202" s="11" t="s">
@@ -11552,7 +11609,7 @@
       <c r="B203" s="21" t="s">
         <v>877</v>
       </c>
-      <c r="C203" s="37" t="s">
+      <c r="C203" s="39" t="s">
         <v>878</v>
       </c>
       <c r="D203" s="19" t="s">
@@ -11587,7 +11644,7 @@
       <c r="B204" s="19" t="s">
         <v>881</v>
       </c>
-      <c r="C204" s="38" t="s">
+      <c r="C204" s="40" t="s">
         <v>882</v>
       </c>
       <c r="D204" s="19" t="s">
@@ -11622,7 +11679,7 @@
       <c r="B205" s="4" t="s">
         <v>887</v>
       </c>
-      <c r="C205" s="53" t="s">
+      <c r="C205" s="55" t="s">
         <v>888</v>
       </c>
       <c r="D205" s="4" t="s">
@@ -11876,19 +11933,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="213">
-      <c r="A213" s="51" t="s">
+      <c r="A213" s="53" t="s">
         <v>915</v>
       </c>
-      <c r="B213" s="51"/>
-      <c r="C213" s="51"/>
-      <c r="D213" s="51"/>
-      <c r="E213" s="51"/>
-      <c r="F213" s="51"/>
-      <c r="G213" s="51"/>
-      <c r="H213" s="51"/>
-      <c r="I213" s="51"/>
-      <c r="J213" s="51"/>
-      <c r="K213" s="51"/>
+      <c r="B213" s="53"/>
+      <c r="C213" s="53"/>
+      <c r="D213" s="53"/>
+      <c r="E213" s="53"/>
+      <c r="F213" s="53"/>
+      <c r="G213" s="53"/>
+      <c r="H213" s="53"/>
+      <c r="I213" s="53"/>
+      <c r="J213" s="53"/>
+      <c r="K213" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="214">
       <c r="A214" s="1" t="s">
@@ -12002,7 +12059,7 @@
       <c r="B217" s="19" t="s">
         <v>636</v>
       </c>
-      <c r="C217" s="55" t="s">
+      <c r="C217" s="57" t="s">
         <v>923</v>
       </c>
       <c r="D217" s="19" t="s">
@@ -12136,19 +12193,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="221">
-      <c r="A221" s="60" t="s">
+      <c r="A221" s="62" t="s">
         <v>942</v>
       </c>
-      <c r="B221" s="60"/>
-      <c r="C221" s="60"/>
-      <c r="D221" s="60"/>
-      <c r="E221" s="60"/>
-      <c r="F221" s="60"/>
-      <c r="G221" s="60"/>
-      <c r="H221" s="60"/>
-      <c r="I221" s="60"/>
-      <c r="J221" s="60"/>
-      <c r="K221" s="60"/>
+      <c r="B221" s="62"/>
+      <c r="C221" s="62"/>
+      <c r="D221" s="62"/>
+      <c r="E221" s="62"/>
+      <c r="F221" s="62"/>
+      <c r="G221" s="62"/>
+      <c r="H221" s="62"/>
+      <c r="I221" s="62"/>
+      <c r="J221" s="62"/>
+      <c r="K221" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="26">

</xml_diff>